<commit_message>
modified the PIIDs for II
</commit_message>
<xml_diff>
--- a/KPMG/Benchmark Appraisal/PIID/II.xlsx
+++ b/KPMG/Benchmark Appraisal/PIID/II.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>II</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>ORG_Project Plan</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>ORG_Design Document</t>
@@ -158,178 +155,13 @@
     <t>Doc</t>
   </si>
   <si>
-    <t>s:project plan of GGE202 verified</t>
-  </si>
-  <si>
-    <t>s:hardware design document of GGE200 verified</t>
-  </si>
-  <si>
-    <t>s: Training is given to team members on different topics</t>
-  </si>
-  <si>
-    <t>s: Policy state that training to be given to update the skills of stakeholders</t>
-  </si>
-  <si>
-    <t>s: updated document are available on SVN</t>
-  </si>
-  <si>
-    <t>s: quality team  ensure to  SM that updated document has been used in project.</t>
-  </si>
-  <si>
-    <t>s: PEG ensure to SM that updated document has been used in project.</t>
-  </si>
-  <si>
-    <t>s: share point used for project repository</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s: Templates and process are available in QMS 3.1 </t>
-  </si>
-  <si>
-    <t>s: project learning available on share point</t>
-  </si>
-  <si>
-    <t>s: process improvement related feedback given by the stakeholder</t>
-  </si>
-  <si>
-    <t>s: process related audit conducted by the PQA team</t>
-  </si>
-  <si>
-    <t>Aff</t>
-  </si>
-  <si>
-    <t>PEG affirmed that he got the training of CMMI model  and resources available to perform the task and policy available on server</t>
-  </si>
-  <si>
-    <t>PPQA affirmed that in audit they verified that stakeholder has used updated documents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEG affirmed that Templates and process are available in QMS 3.1 and share point used for project repository </t>
-  </si>
-  <si>
-    <t>PQA affirmed that audit of audit function done in regular intervals</t>
-  </si>
-  <si>
-    <t>PEG affirmed that Process improvement proposals use to improve process and templates</t>
-  </si>
-  <si>
-    <t>PQA affirmed that he got the training and having resource issue and escalated to PEG and SM and policy available on server</t>
-  </si>
-  <si>
-    <t>PEG affirmed that updated process and template are available on server</t>
-  </si>
-  <si>
-    <t>PEG affirmed that project team use different templates which are released in QMS for project activities</t>
-  </si>
-  <si>
-    <t>PQA affirmed that use different templates which are released in QMS for his PQA activities</t>
-  </si>
-  <si>
-    <t>PM1 affirmed that project team use different templates which are released in QMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM2 affirmed that project team use different templates which are released in QMS </t>
-  </si>
-  <si>
-    <t>PM3 affirmed that project team use different templates which are released in QMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM4 affirmed that project team use different templates which are released in QMS </t>
-  </si>
-  <si>
-    <t>SM affirmed that project team use different templates available on  QMS</t>
-  </si>
-  <si>
     <t>Released QMS to use organizational process assets</t>
   </si>
   <si>
     <t>PQA Plan (Audit plan) means organization process adherence and effectiveness perform and manage.</t>
   </si>
   <si>
-    <t>PM1 affirmed that team has received training on QMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM2 affirmed that team has received training on QMS and on SMF battery </t>
-  </si>
-  <si>
-    <t>PM3 affirmed that team has received training on QMS</t>
-  </si>
-  <si>
-    <t>PM4 affirmed that team has received training on QMS</t>
-  </si>
-  <si>
-    <t>SM affirmed that training is given to team to perform  activities</t>
-  </si>
-  <si>
-    <t>PM1 affirmed that updated documents are available on QMS3.1</t>
-  </si>
-  <si>
-    <t>PM2 affirmed that updated documents are available on QMS3.1</t>
-  </si>
-  <si>
-    <t>PM3 affirmed that updated documents are available on QMS3.1</t>
-  </si>
-  <si>
-    <t>PM4 affirmed that updated documents are available on QMS3.1</t>
-  </si>
-  <si>
-    <t>SM affirmed that documents are available on project server</t>
-  </si>
-  <si>
-    <t>PM1 affirmed that Templates and process are available in QMS 3.1 and share point used for project repository</t>
-  </si>
-  <si>
-    <t>PQA affirmed that Templates and process are available in QMS 3.1 and share point used for his activities</t>
-  </si>
-  <si>
-    <t>PM2 affirmed that Templates and process are available in QMS 3.1 and share point used for project repository</t>
-  </si>
-  <si>
-    <t>PM3 affirmed that Templates and process are available in QMS 3.1 and share point used for project repository</t>
-  </si>
-  <si>
-    <t>PM4 affirmed that Templates and process are available in QMS 3.1 and share point used for project repository</t>
-  </si>
-  <si>
-    <t>SM affirmed that Templates and process are available in QMS 3.1 and share point used for project repository</t>
-  </si>
-  <si>
-    <t>PM1 affirmed that audit of his project has been done</t>
-  </si>
-  <si>
-    <t>PM2 affirmed that audit of his project has been done</t>
-  </si>
-  <si>
-    <t>PM3 affirmed that audit of his project has been done</t>
-  </si>
-  <si>
-    <t>PM4 affirmed that audit of his project has been done</t>
-  </si>
-  <si>
-    <t>SM affirmed that we review the Audit report</t>
-  </si>
-  <si>
-    <t>PM1 affirmed that his team has given suggestion to improve process assets during project life cycle</t>
-  </si>
-  <si>
-    <t>PM2 affirmed that his team has given suggestion to improve process assets during project life cycle</t>
-  </si>
-  <si>
-    <t>PM3 affirmed that his team has given suggestion to improve process assets during project life cycle</t>
-  </si>
-  <si>
-    <t>PM4 affirmed that his team has given suggestion to improve process assets during project life cycle</t>
-  </si>
-  <si>
-    <t>SM affirmed that project learning available on SharePoint</t>
-  </si>
-  <si>
     <t>PQA reviews ensure developed process followed by practitioner</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>Project SP10 GGE302 Project plan as example work product shows perform processes.</t>
   </si>
   <si>
     <t>Project GGE295 hardware design document as example work product shows perform processes.</t>
@@ -344,16 +176,46 @@
     <t>Einframe also as organization assets which use to perform work.</t>
   </si>
   <si>
-    <t>PEG affirmed that audit of his activities has been done on 3 months bases</t>
-  </si>
-  <si>
-    <t>Einframe capture incident site use to capture process improvement suggestions, Process improvement proposals use to contribute process related suggestions and these taken as input to improve process assets.</t>
-  </si>
-  <si>
     <t>ORG_Approved_Learning</t>
   </si>
   <si>
-    <t>Approved learnings site use to improve process assets.</t>
+    <t>Project GGE302 Project plan as example work product shows perform processes.</t>
+  </si>
+  <si>
+    <t>PEG plan contains budget, resources provided by senior management to develop and maintain processes.</t>
+  </si>
+  <si>
+    <t>ORG_PEG_PLAN</t>
+  </si>
+  <si>
+    <t>ORG_Einframe_Resource</t>
+  </si>
+  <si>
+    <t>Approval on quotation for Einframe as resource for process implementation.</t>
+  </si>
+  <si>
+    <t>ORG_Einframe_Process_Reviews</t>
+  </si>
+  <si>
+    <t>Processes reviews with team to ensure the team follow the process, and discussed and took understanding sessions.</t>
+  </si>
+  <si>
+    <t>ORG_MBR_Review_MINMET</t>
+  </si>
+  <si>
+    <t>Minutes of meeting of MBR review meeting with senior management to evaluate the processes effectiveness.</t>
+  </si>
+  <si>
+    <t>Approved learnings in Einframe captured best proactices, good or bad learnings etc.</t>
+  </si>
+  <si>
+    <t>Einframe capture incident use to capture process improvement suggestions, Process improvement proposals use to contribute process related suggestions and these taken as input to improve process assets.</t>
+  </si>
+  <si>
+    <t>ORG_HW_Library</t>
+  </si>
+  <si>
+    <t>Master library captured technical modules for future use.</t>
   </si>
 </sst>
 </file>
@@ -476,18 +338,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -615,7 +471,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -825,9 +681,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1281,7 +1134,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F81" sqref="F81"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1378,21 +1231,17 @@
         <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H4" s="4"/>
       <c r="I4" s="8" t="str">
         <f>IF(MID(H4,2,1)=":",LEFT(H4,1),"-")</f>
-        <v>s</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J4" s="8"/>
       <c r="K4" s="7" t="str">
         <f>IF(COUNTIFS($E4,"*"&amp;K$3&amp;"*")&gt;=1,"X","")</f>
         <v>X</v>
@@ -1405,9 +1254,7 @@
         <f t="shared" si="0"/>
         <v>X</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>94</v>
-      </c>
+      <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="61"/>
@@ -1422,24 +1269,20 @@
         <v>OK</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H5" s="4"/>
       <c r="I5" s="8" t="str">
         <f t="shared" ref="I5:I68" si="2">IF(MID(H5,2,1)=":",LEFT(H5,1),"-")</f>
-        <v>s</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J5" s="8"/>
       <c r="K5" s="7" t="str">
         <f t="shared" ref="K5:M68" si="3">IF(COUNTIFS($E5,"*"&amp;K$3&amp;"*")&gt;=1,"X","")</f>
         <v>X</v>
@@ -1458,7 +1301,7 @@
       <c r="Q5" s="62"/>
       <c r="R5" s="68"/>
     </row>
-    <row r="6" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="68"/>
       <c r="B6" s="62"/>
       <c r="C6" s="58"/>
@@ -1467,20 +1310,14 @@
         <v>-</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J6" s="8"/>
       <c r="K6" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1499,7 +1336,7 @@
       <c r="Q6" s="62"/>
       <c r="R6" s="68"/>
     </row>
-    <row r="7" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="68"/>
       <c r="B7" s="62"/>
       <c r="C7" s="58"/>
@@ -1508,20 +1345,14 @@
         <v>-</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F7" s="54"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="4"/>
       <c r="I7" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J7" s="8"/>
       <c r="K7" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1540,7 +1371,7 @@
       <c r="Q7" s="62"/>
       <c r="R7" s="68"/>
     </row>
-    <row r="8" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="68"/>
       <c r="B8" s="62"/>
       <c r="C8" s="58"/>
@@ -1549,20 +1380,14 @@
         <v>-</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="4"/>
       <c r="I8" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J8" s="8"/>
       <c r="K8" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1581,7 +1406,7 @@
       <c r="Q8" s="62"/>
       <c r="R8" s="68"/>
     </row>
-    <row r="9" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="68"/>
       <c r="B9" s="62"/>
       <c r="C9" s="58"/>
@@ -1590,20 +1415,14 @@
         <v>-</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="4"/>
       <c r="I9" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J9" s="8"/>
       <c r="K9" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1622,7 +1441,7 @@
       <c r="Q9" s="62"/>
       <c r="R9" s="68"/>
     </row>
-    <row r="10" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="68"/>
       <c r="B10" s="62"/>
       <c r="C10" s="58"/>
@@ -1631,20 +1450,14 @@
         <v>-</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="4"/>
       <c r="I10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J10" s="8"/>
       <c r="K10" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1663,7 +1476,7 @@
       <c r="Q10" s="62"/>
       <c r="R10" s="68"/>
     </row>
-    <row r="11" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="68"/>
       <c r="B11" s="62"/>
       <c r="C11" s="58"/>
@@ -1672,20 +1485,14 @@
         <v>-</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="4"/>
       <c r="I11" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J11" s="8"/>
       <c r="K11" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1704,7 +1511,7 @@
       <c r="Q11" s="62"/>
       <c r="R11" s="68"/>
     </row>
-    <row r="12" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="68"/>
       <c r="B12" s="62"/>
       <c r="C12" s="58"/>
@@ -1713,20 +1520,14 @@
         <v>-</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="4"/>
       <c r="I12" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J12" s="8"/>
       <c r="K12" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1957,37 +1758,33 @@
     </row>
     <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A19" s="68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="61">
         <v>2.1</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H19" s="4"/>
       <c r="I19" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J19" s="8"/>
       <c r="K19" s="7" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -2000,9 +1797,7 @@
         <f t="shared" si="0"/>
         <v>X</v>
       </c>
-      <c r="N19" s="7" t="s">
-        <v>94</v>
-      </c>
+      <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="61"/>
@@ -2017,24 +1812,20 @@
         <v>OK</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="G20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H20" s="4"/>
       <c r="I20" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J20" s="8"/>
       <c r="K20" s="7" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -2053,40 +1844,40 @@
       <c r="Q20" s="62"/>
       <c r="R20" s="68"/>
     </row>
-    <row r="21" spans="1:18" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A21" s="68"/>
       <c r="B21" s="62"/>
       <c r="C21" s="60"/>
       <c r="D21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E21" s="5"/>
+        <v>OK</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="F21" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J21" s="8"/>
       <c r="K21" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L21" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M21" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
@@ -2094,40 +1885,40 @@
       <c r="Q21" s="62"/>
       <c r="R21" s="68"/>
     </row>
-    <row r="22" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="68"/>
       <c r="B22" s="62"/>
       <c r="C22" s="60"/>
       <c r="D22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E22" s="5"/>
+        <v>OK</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="F22" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J22" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J22" s="8"/>
       <c r="K22" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L22" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M22" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -2135,7 +1926,7 @@
       <c r="Q22" s="62"/>
       <c r="R22" s="68"/>
     </row>
-    <row r="23" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="68"/>
       <c r="B23" s="62"/>
       <c r="C23" s="60"/>
@@ -2144,20 +1935,14 @@
         <v>-</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="4"/>
       <c r="I23" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J23" s="8"/>
       <c r="K23" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2176,7 +1961,7 @@
       <c r="Q23" s="62"/>
       <c r="R23" s="68"/>
     </row>
-    <row r="24" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="68"/>
       <c r="B24" s="62"/>
       <c r="C24" s="60"/>
@@ -2185,20 +1970,14 @@
         <v>-</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
       <c r="H24" s="4"/>
       <c r="I24" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J24" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J24" s="8"/>
       <c r="K24" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2217,7 +1996,7 @@
       <c r="Q24" s="62"/>
       <c r="R24" s="68"/>
     </row>
-    <row r="25" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="68"/>
       <c r="B25" s="62"/>
       <c r="C25" s="60"/>
@@ -2226,20 +2005,14 @@
         <v>-</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="4"/>
       <c r="I25" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J25" s="8"/>
       <c r="K25" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2267,20 +2040,14 @@
         <v>-</v>
       </c>
       <c r="E26" s="6"/>
-      <c r="F26" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="4"/>
       <c r="I26" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J26" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J26" s="8"/>
       <c r="K26" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2299,7 +2066,7 @@
       <c r="Q26" s="62"/>
       <c r="R26" s="68"/>
     </row>
-    <row r="27" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="68"/>
       <c r="B27" s="62"/>
       <c r="C27" s="60"/>
@@ -2308,20 +2075,14 @@
         <v>-</v>
       </c>
       <c r="E27" s="6"/>
-      <c r="F27" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="7"/>
       <c r="H27" s="4"/>
       <c r="I27" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J27" s="8"/>
       <c r="K27" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2556,31 +2317,27 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C34" s="60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" s="4" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
       <c r="E34" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="G34" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H34" s="4"/>
       <c r="I34" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J34" s="8"/>
       <c r="K34" s="7" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -2593,15 +2350,13 @@
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="N34" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="N34" s="10"/>
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="61"/>
       <c r="R34" s="68"/>
     </row>
-    <row r="35" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" s="68"/>
       <c r="B35" s="62"/>
       <c r="C35" s="60"/>
@@ -2609,25 +2364,21 @@
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="E35" s="70" t="s">
-        <v>28</v>
+      <c r="E35" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H35" s="4"/>
       <c r="I35" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J35" s="8"/>
       <c r="K35" s="7" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -2646,7 +2397,7 @@
       <c r="Q35" s="62"/>
       <c r="R35" s="68"/>
     </row>
-    <row r="36" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A36" s="68"/>
       <c r="B36" s="62"/>
       <c r="C36" s="60"/>
@@ -2655,24 +2406,20 @@
         <v>OK</v>
       </c>
       <c r="E36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="G36" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H36" s="4"/>
       <c r="I36" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J36" s="8"/>
       <c r="K36" s="7" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -2691,40 +2438,40 @@
       <c r="Q36" s="62"/>
       <c r="R36" s="68"/>
     </row>
-    <row r="37" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A37" s="68"/>
       <c r="B37" s="62"/>
       <c r="C37" s="60"/>
       <c r="D37" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E37" s="5"/>
+        <v>OK</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="F37" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J37" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J37" s="8"/>
       <c r="K37" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L37" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M37" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
@@ -2732,7 +2479,7 @@
       <c r="Q37" s="62"/>
       <c r="R37" s="68"/>
     </row>
-    <row r="38" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="68"/>
       <c r="B38" s="62"/>
       <c r="C38" s="60"/>
@@ -2741,20 +2488,14 @@
         <v>-</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="10"/>
       <c r="H38" s="4"/>
       <c r="I38" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J38" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J38" s="8"/>
       <c r="K38" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2773,7 +2514,7 @@
       <c r="Q38" s="62"/>
       <c r="R38" s="68"/>
     </row>
-    <row r="39" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="68"/>
       <c r="B39" s="62"/>
       <c r="C39" s="60"/>
@@ -2782,20 +2523,14 @@
         <v>-</v>
       </c>
       <c r="E39" s="5"/>
-      <c r="F39" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="10"/>
       <c r="H39" s="4"/>
       <c r="I39" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J39" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J39" s="8"/>
       <c r="K39" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2814,7 +2549,7 @@
       <c r="Q39" s="62"/>
       <c r="R39" s="68"/>
     </row>
-    <row r="40" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="68"/>
       <c r="B40" s="62"/>
       <c r="C40" s="60"/>
@@ -2823,20 +2558,14 @@
         <v>-</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="F40" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="4"/>
       <c r="I40" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J40" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J40" s="8"/>
       <c r="K40" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2855,7 +2584,7 @@
       <c r="Q40" s="62"/>
       <c r="R40" s="68"/>
     </row>
-    <row r="41" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="68"/>
       <c r="B41" s="62"/>
       <c r="C41" s="60"/>
@@ -2864,20 +2593,14 @@
         <v>-</v>
       </c>
       <c r="E41" s="6"/>
-      <c r="F41" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="10"/>
       <c r="H41" s="4"/>
       <c r="I41" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J41" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J41" s="8"/>
       <c r="K41" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2896,7 +2619,7 @@
       <c r="Q41" s="62"/>
       <c r="R41" s="68"/>
     </row>
-    <row r="42" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="68"/>
       <c r="B42" s="62"/>
       <c r="C42" s="60"/>
@@ -2905,20 +2628,14 @@
         <v>-</v>
       </c>
       <c r="E42" s="6"/>
-      <c r="F42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="4"/>
       <c r="I42" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J42" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J42" s="8"/>
       <c r="K42" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2937,7 +2654,7 @@
       <c r="Q42" s="62"/>
       <c r="R42" s="68"/>
     </row>
-    <row r="43" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="68"/>
       <c r="B43" s="62"/>
       <c r="C43" s="60"/>
@@ -2946,20 +2663,14 @@
         <v>-</v>
       </c>
       <c r="E43" s="6"/>
-      <c r="F43" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="10"/>
       <c r="H43" s="4"/>
       <c r="I43" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J43" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J43" s="8"/>
       <c r="K43" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3155,37 +2866,33 @@
     </row>
     <row r="49" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="68" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" s="61">
         <v>3.1</v>
       </c>
       <c r="C49" s="60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D49" s="4" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H49" s="4"/>
       <c r="I49" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J49" s="8"/>
       <c r="K49" s="7" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -3198,9 +2905,7 @@
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="N49" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="N49" s="10"/>
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
       <c r="Q49" s="61"/>
@@ -3215,24 +2920,20 @@
         <v>OK</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H50" s="4"/>
       <c r="I50" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J50" s="8"/>
       <c r="K50" s="7" t="str">
         <f>IF(COUNTIFS($E50,"*"&amp;K$3&amp;"*")&gt;=1,"X","")</f>
         <v>X</v>
@@ -3251,7 +2952,7 @@
       <c r="Q50" s="62"/>
       <c r="R50" s="68"/>
     </row>
-    <row r="51" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="68"/>
       <c r="B51" s="62"/>
       <c r="C51" s="60"/>
@@ -3260,20 +2961,14 @@
         <v>-</v>
       </c>
       <c r="E51" s="5"/>
-      <c r="F51" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="10"/>
       <c r="H51" s="4"/>
       <c r="I51" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J51" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J51" s="8"/>
       <c r="K51" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3292,7 +2987,7 @@
       <c r="Q51" s="62"/>
       <c r="R51" s="68"/>
     </row>
-    <row r="52" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="68"/>
       <c r="B52" s="62"/>
       <c r="C52" s="60"/>
@@ -3301,20 +2996,14 @@
         <v>-</v>
       </c>
       <c r="E52" s="5"/>
-      <c r="F52" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="10"/>
       <c r="H52" s="4"/>
       <c r="I52" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J52" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J52" s="8"/>
       <c r="K52" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3333,7 +3022,7 @@
       <c r="Q52" s="62"/>
       <c r="R52" s="68"/>
     </row>
-    <row r="53" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="68"/>
       <c r="B53" s="62"/>
       <c r="C53" s="60"/>
@@ -3342,20 +3031,14 @@
         <v>-</v>
       </c>
       <c r="E53" s="5"/>
-      <c r="F53" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="10"/>
       <c r="H53" s="4"/>
       <c r="I53" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J53" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J53" s="8"/>
       <c r="K53" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3374,7 +3057,7 @@
       <c r="Q53" s="62"/>
       <c r="R53" s="68"/>
     </row>
-    <row r="54" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="68"/>
       <c r="B54" s="62"/>
       <c r="C54" s="60"/>
@@ -3383,20 +3066,14 @@
         <v>-</v>
       </c>
       <c r="E54" s="5"/>
-      <c r="F54" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="10"/>
       <c r="H54" s="4"/>
       <c r="I54" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J54" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J54" s="8"/>
       <c r="K54" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3415,7 +3092,7 @@
       <c r="Q54" s="62"/>
       <c r="R54" s="68"/>
     </row>
-    <row r="55" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="68"/>
       <c r="B55" s="62"/>
       <c r="C55" s="60"/>
@@ -3424,20 +3101,14 @@
         <v>-</v>
       </c>
       <c r="E55" s="6"/>
-      <c r="F55" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="10"/>
       <c r="H55" s="4"/>
       <c r="I55" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J55" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J55" s="8"/>
       <c r="K55" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3456,7 +3127,7 @@
       <c r="Q55" s="62"/>
       <c r="R55" s="68"/>
     </row>
-    <row r="56" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="68"/>
       <c r="B56" s="62"/>
       <c r="C56" s="60"/>
@@ -3465,20 +3136,14 @@
         <v>-</v>
       </c>
       <c r="E56" s="6"/>
-      <c r="F56" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="10"/>
       <c r="H56" s="4"/>
       <c r="I56" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J56" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J56" s="8"/>
       <c r="K56" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3497,7 +3162,7 @@
       <c r="Q56" s="62"/>
       <c r="R56" s="68"/>
     </row>
-    <row r="57" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="68"/>
       <c r="B57" s="62"/>
       <c r="C57" s="60"/>
@@ -3506,20 +3171,14 @@
         <v>-</v>
       </c>
       <c r="E57" s="6"/>
-      <c r="F57" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="10"/>
       <c r="H57" s="4"/>
       <c r="I57" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J57" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J57" s="8"/>
       <c r="K57" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3754,31 +3413,27 @@
         <v>3.2</v>
       </c>
       <c r="C64" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D64" s="4" t="str">
         <f>IF(LEN(E64)&gt;5,IF(LEN(K64&amp;L64&amp;M64)&gt;=1,"OK","Check"),"-")</f>
         <v>OK</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H64" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H64" s="4"/>
       <c r="I64" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>s</v>
-      </c>
-      <c r="J64" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J64" s="8"/>
       <c r="K64" s="7" t="str">
         <f>IF(COUNTIFS($E64,"*"&amp;K$3&amp;"*")&gt;=1,"X","")</f>
         <v>X</v>
@@ -3791,48 +3446,46 @@
         <f>IF(COUNTIFS($E64,"*"&amp;M$3&amp;"*")&gt;=1,"X","")</f>
         <v>X</v>
       </c>
-      <c r="N64" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="N64" s="10"/>
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
       <c r="Q64" s="61"/>
       <c r="R64" s="68"/>
     </row>
-    <row r="65" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A65" s="68"/>
       <c r="B65" s="68"/>
       <c r="C65" s="60"/>
       <c r="D65" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E65" s="9"/>
+        <v>OK</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="F65" s="6" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J65" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J65" s="8"/>
       <c r="K65" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L65" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M65" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N65" s="10"/>
       <c r="O65" s="10"/>
@@ -3840,7 +3493,7 @@
       <c r="Q65" s="62"/>
       <c r="R65" s="68"/>
     </row>
-    <row r="66" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="68"/>
       <c r="B66" s="68"/>
       <c r="C66" s="60"/>
@@ -3849,20 +3502,14 @@
         <v>-</v>
       </c>
       <c r="E66" s="5"/>
-      <c r="F66" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G66" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F66" s="6"/>
+      <c r="G66" s="10"/>
       <c r="H66" s="4"/>
       <c r="I66" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J66" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J66" s="8"/>
       <c r="K66" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3881,7 +3528,7 @@
       <c r="Q66" s="62"/>
       <c r="R66" s="68"/>
     </row>
-    <row r="67" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="68"/>
       <c r="B67" s="68"/>
       <c r="C67" s="60"/>
@@ -3890,20 +3537,14 @@
         <v>-</v>
       </c>
       <c r="E67" s="5"/>
-      <c r="F67" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F67" s="6"/>
+      <c r="G67" s="10"/>
       <c r="H67" s="4"/>
       <c r="I67" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J67" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J67" s="8"/>
       <c r="K67" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3922,7 +3563,7 @@
       <c r="Q67" s="62"/>
       <c r="R67" s="68"/>
     </row>
-    <row r="68" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="68"/>
       <c r="B68" s="68"/>
       <c r="C68" s="60"/>
@@ -3931,20 +3572,14 @@
         <v>-</v>
       </c>
       <c r="E68" s="5"/>
-      <c r="F68" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G68" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="10"/>
       <c r="H68" s="4"/>
       <c r="I68" s="8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="J68" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J68" s="8"/>
       <c r="K68" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3963,7 +3598,7 @@
       <c r="Q68" s="62"/>
       <c r="R68" s="68"/>
     </row>
-    <row r="69" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="68"/>
       <c r="B69" s="68"/>
       <c r="C69" s="60"/>
@@ -3972,20 +3607,14 @@
         <v>-</v>
       </c>
       <c r="E69" s="5"/>
-      <c r="F69" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G69" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F69" s="6"/>
+      <c r="G69" s="10"/>
       <c r="H69" s="4"/>
       <c r="I69" s="8" t="str">
         <f t="shared" ref="I69:I132" si="5">IF(MID(H69,2,1)=":",LEFT(H69,1),"-")</f>
         <v>-</v>
       </c>
-      <c r="J69" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J69" s="8"/>
       <c r="K69" s="7" t="str">
         <f t="shared" ref="K69:M132" si="6">IF(COUNTIFS($E69,"*"&amp;K$3&amp;"*")&gt;=1,"X","")</f>
         <v/>
@@ -4004,7 +3633,7 @@
       <c r="Q69" s="62"/>
       <c r="R69" s="68"/>
     </row>
-    <row r="70" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="68"/>
       <c r="B70" s="68"/>
       <c r="C70" s="60"/>
@@ -4013,20 +3642,14 @@
         <v>-</v>
       </c>
       <c r="E70" s="6"/>
-      <c r="F70" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F70" s="6"/>
+      <c r="G70" s="10"/>
       <c r="H70" s="4"/>
       <c r="I70" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J70" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J70" s="8"/>
       <c r="K70" s="7" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4045,7 +3668,7 @@
       <c r="Q70" s="62"/>
       <c r="R70" s="68"/>
     </row>
-    <row r="71" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="68"/>
       <c r="B71" s="68"/>
       <c r="C71" s="60"/>
@@ -4054,20 +3677,14 @@
         <v>-</v>
       </c>
       <c r="E71" s="6"/>
-      <c r="F71" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F71" s="6"/>
+      <c r="G71" s="10"/>
       <c r="H71" s="4"/>
       <c r="I71" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J71" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J71" s="8"/>
       <c r="K71" s="7" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4337,31 +3954,27 @@
         <v>3.3</v>
       </c>
       <c r="C79" s="60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D79" s="4" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H79" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H79" s="4"/>
       <c r="I79" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>s</v>
-      </c>
-      <c r="J79" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J79" s="8"/>
       <c r="K79" s="7" t="str">
         <f t="shared" si="6"/>
         <v>X</v>
@@ -4374,15 +3987,13 @@
         <f t="shared" si="6"/>
         <v>X</v>
       </c>
-      <c r="N79" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="N79" s="10"/>
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
       <c r="Q79" s="61"/>
       <c r="R79" s="68"/>
     </row>
-    <row r="80" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A80" s="68"/>
       <c r="B80" s="68"/>
       <c r="C80" s="60"/>
@@ -4391,24 +4002,20 @@
         <v>OK</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H80" s="4"/>
       <c r="I80" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>s</v>
-      </c>
-      <c r="J80" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>-</v>
+      </c>
+      <c r="J80" s="8"/>
       <c r="K80" s="7" t="str">
         <f t="shared" si="6"/>
         <v>X</v>
@@ -4427,40 +4034,40 @@
       <c r="Q80" s="62"/>
       <c r="R80" s="68"/>
     </row>
-    <row r="81" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" s="68"/>
       <c r="B81" s="68"/>
       <c r="C81" s="60"/>
       <c r="D81" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-      <c r="E81" s="5"/>
+        <v>OK</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="F81" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J81" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J81" s="8"/>
       <c r="K81" s="7" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L81" s="7" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M81" s="7" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N81" s="10"/>
       <c r="O81" s="10"/>
@@ -4468,7 +4075,7 @@
       <c r="Q81" s="62"/>
       <c r="R81" s="68"/>
     </row>
-    <row r="82" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="68"/>
       <c r="B82" s="68"/>
       <c r="C82" s="60"/>
@@ -4477,20 +4084,14 @@
         <v>-</v>
       </c>
       <c r="E82" s="5"/>
-      <c r="F82" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F82" s="6"/>
+      <c r="G82" s="10"/>
       <c r="H82" s="4"/>
       <c r="I82" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J82" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J82" s="8"/>
       <c r="K82" s="7" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4509,7 +4110,7 @@
       <c r="Q82" s="62"/>
       <c r="R82" s="68"/>
     </row>
-    <row r="83" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="68"/>
       <c r="B83" s="68"/>
       <c r="C83" s="60"/>
@@ -4518,20 +4119,14 @@
         <v>-</v>
       </c>
       <c r="E83" s="6"/>
-      <c r="F83" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F83" s="6"/>
+      <c r="G83" s="10"/>
       <c r="H83" s="4"/>
       <c r="I83" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J83" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J83" s="8"/>
       <c r="K83" s="7" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4550,7 +4145,7 @@
       <c r="Q83" s="62"/>
       <c r="R83" s="68"/>
     </row>
-    <row r="84" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="68"/>
       <c r="B84" s="68"/>
       <c r="C84" s="60"/>
@@ -4559,20 +4154,14 @@
         <v>-</v>
       </c>
       <c r="E84" s="6"/>
-      <c r="F84" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F84" s="6"/>
+      <c r="G84" s="10"/>
       <c r="H84" s="4"/>
       <c r="I84" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J84" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J84" s="8"/>
       <c r="K84" s="7" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4591,7 +4180,7 @@
       <c r="Q84" s="62"/>
       <c r="R84" s="68"/>
     </row>
-    <row r="85" spans="1:18" ht="51" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="68"/>
       <c r="B85" s="68"/>
       <c r="C85" s="60"/>
@@ -4600,20 +4189,14 @@
         <v>-</v>
       </c>
       <c r="E85" s="12"/>
-      <c r="F85" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G85" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F85" s="6"/>
+      <c r="G85" s="10"/>
       <c r="H85" s="4"/>
       <c r="I85" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J85" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J85" s="8"/>
       <c r="K85" s="7" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4632,7 +4215,7 @@
       <c r="Q85" s="62"/>
       <c r="R85" s="68"/>
     </row>
-    <row r="86" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="68"/>
       <c r="B86" s="68"/>
       <c r="C86" s="60"/>
@@ -4641,20 +4224,14 @@
         <v>-</v>
       </c>
       <c r="E86" s="6"/>
-      <c r="F86" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F86" s="6"/>
+      <c r="G86" s="10"/>
       <c r="H86" s="4"/>
       <c r="I86" s="8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="J86" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J86" s="8"/>
       <c r="K86" s="7" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -8390,7 +7967,7 @@
       <c r="G193" s="10"/>
       <c r="H193" s="4"/>
       <c r="I193" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J193" s="8"/>
       <c r="K193" s="7" t="str">
@@ -11226,7 +10803,7 @@
     </row>
     <row r="275" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B275" s="52"/>
       <c r="C275" s="52"/>
@@ -11424,7 +11001,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E19" r:id="rId1"/>
-    <hyperlink ref="E35" r:id="rId2" display="PQA SM review"/>
+    <hyperlink ref="E35" r:id="rId2"/>
     <hyperlink ref="E80" r:id="rId3" display="ORG_Project Learning Log"/>
     <hyperlink ref="E64" r:id="rId4"/>
     <hyperlink ref="E4" r:id="rId5"/>
@@ -11435,9 +11012,14 @@
     <hyperlink ref="E49" r:id="rId10"/>
     <hyperlink ref="E50" r:id="rId11"/>
     <hyperlink ref="E79" r:id="rId12"/>
+    <hyperlink ref="E21" r:id="rId13"/>
+    <hyperlink ref="E22" r:id="rId14"/>
+    <hyperlink ref="E37" r:id="rId15"/>
+    <hyperlink ref="E65" r:id="rId16"/>
+    <hyperlink ref="E81" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;P&amp;R&amp;A</oddHeader>
   </headerFooter>

</xml_diff>